<commit_message>
Add writhing into Excel report from MySql.
</commit_message>
<xml_diff>
--- a/Generated-Reports/Excel-report.xlsx
+++ b/Generated-Reports/Excel-report.xlsx
@@ -24,15 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Trips Excel Report</t>
   </si>
   <si>
-    <t>Trip Name</t>
-  </si>
-  <si>
-    <t>Country</t>
+    <t>Trip Name (from SQLite)</t>
+  </si>
+  <si>
+    <t>Country (from SQLite)</t>
+  </si>
+  <si>
+    <t>Touroperator (from MySQL)</t>
+  </si>
+  <si>
+    <t>Trips Sold (from MySQL)</t>
+  </si>
+  <si>
+    <t>Income (from MySQL)</t>
   </si>
   <si>
     <t>Italy The One And Only</t>
@@ -41,16 +50,16 @@
     <t>Europe</t>
   </si>
   <si>
-    <t>Mie Perfecture Japan</t>
-  </si>
-  <si>
-    <t>Asia</t>
+    <t>Eleganca Tours</t>
   </si>
   <si>
     <t>The Secret Beauty Of Mexico</t>
   </si>
   <si>
     <t>North America</t>
+  </si>
+  <si>
+    <t>Elite Travel Agency</t>
   </si>
   <si>
     <t>Chiloe Chile</t>
@@ -106,15 +115,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,66 +412,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="25.77734375" customWidth="1"/>
+    <col min="1" max="5" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>12672</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>40920</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
+      <c r="E5">
+        <v>25800</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated data in Sqlite
</commit_message>
<xml_diff>
--- a/Generated-Reports/Excel-report.xlsx
+++ b/Generated-Reports/Excel-report.xlsx
@@ -1,30 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\06. Telerik\00 - Teamworks\04 - TravelAgency\Team-French-75\Generated-Reports\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10476" windowHeight="3972"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="14355" windowHeight="4185"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Trips Excel Report</t>
   </si>
@@ -53,19 +45,115 @@
     <t>Eleganca Tours</t>
   </si>
   <si>
+    <t>Lefkada The Emerald Island</t>
+  </si>
+  <si>
+    <t>Mie Prefecture Japan</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
     <t>The Secret Beauty Of Mexico</t>
   </si>
   <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Elite Travel Agency</t>
+  </si>
+  <si>
+    <t>Chiloe Chile</t>
+  </si>
+  <si>
+    <t>Liege Belgium</t>
+  </si>
+  <si>
+    <t>Santorini Holiday</t>
+  </si>
+  <si>
+    <t>Mirage Travel</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Rea Holidays</t>
+  </si>
+  <si>
+    <t>Sicily Italy</t>
+  </si>
+  <si>
+    <t>Mega Travel</t>
+  </si>
+  <si>
+    <t>Tasmania</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
     <t>North America</t>
   </si>
   <si>
-    <t>Elite Travel Agency</t>
-  </si>
-  <si>
-    <t>Chiloe Chile</t>
-  </si>
-  <si>
-    <t>South America</t>
+    <t>Reina Travel</t>
+  </si>
+  <si>
+    <t>Galle Sri Lanka</t>
+  </si>
+  <si>
+    <t>Alma Travel</t>
+  </si>
+  <si>
+    <t>Zagreb Croatia</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>New Balkan Tours</t>
+  </si>
+  <si>
+    <t>West Bay Beach</t>
+  </si>
+  <si>
+    <t>Avioturs</t>
+  </si>
+  <si>
+    <t>Torres Del Paine</t>
+  </si>
+  <si>
+    <t>Classic Journeys</t>
+  </si>
+  <si>
+    <t>Baia do Sancho</t>
+  </si>
+  <si>
+    <t>Daria Travel</t>
+  </si>
+  <si>
+    <t>Instanbul</t>
+  </si>
+  <si>
+    <t>Europe and Asia</t>
+  </si>
+  <si>
+    <t>Gray &amp; Co</t>
+  </si>
+  <si>
+    <t>Bora Bora</t>
+  </si>
+  <si>
+    <t>Island</t>
+  </si>
+  <si>
+    <t>Absolute Travel</t>
   </si>
 </sst>
 </file>
@@ -78,7 +166,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -134,7 +221,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -142,17 +229,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -160,39 +244,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,7 +346,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -271,159 +355,183 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="25.77734375" customWidth="1"/>
+    <col min="1" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +540,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -449,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -466,38 +574,310 @@
         <v>12672</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4">
+        <v>3264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>23250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="E4">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
         <v>40920</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>25800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="E9">
+        <v>5970</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="E5">
-        <v>25800</v>
+      <c r="E10">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>28700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>28900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>28080</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>4680</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>8580</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>33950</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>34320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>31030</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20">
+        <v>13</v>
+      </c>
+      <c r="E20">
+        <v>9495</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>39220</v>
       </c>
     </row>
   </sheetData>
@@ -505,6 +885,30 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>